<commit_message>
Updated data set ffa.
</commit_message>
<xml_diff>
--- a/src/original_data/FRB_Z1.xlsx
+++ b/src/original_data/FRB_Z1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="289">
   <si>
     <t>Download Page</t>
   </si>
@@ -883,6 +883,9 @@
   </si>
   <si>
     <t>2015Q2</t>
+  </si>
+  <si>
+    <t>2015Q3</t>
   </si>
 </sst>
 </file>
@@ -1293,7 +1296,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I261"/>
+  <dimension ref="A1:I262"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -8848,6 +8851,35 @@
       </c>
       <c r="I261">
         <v>305512</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9">
+      <c r="A262" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B262">
+        <v>585851</v>
+      </c>
+      <c r="C262">
+        <v>-668476</v>
+      </c>
+      <c r="D262">
+        <v>580409</v>
+      </c>
+      <c r="E262">
+        <v>5272</v>
+      </c>
+      <c r="F262">
+        <v>22332</v>
+      </c>
+      <c r="G262">
+        <v>2122468</v>
+      </c>
+      <c r="H262">
+        <v>1332701</v>
+      </c>
+      <c r="I262">
+        <v>308860</v>
       </c>
     </row>
   </sheetData>

</xml_diff>